<commit_message>
[BI-1867] - Ontology: Increase name length to 16 characters
</commit_message>
<xml_diff>
--- a/src/files/TraitImport/test_traits_exceedsCharLen.xlsx
+++ b/src/files/TraitImport/test_traits_exceedsCharLen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hms243/IdeaProjects/taf/src/files/TraitImport/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF12A336-6FF9-0F41-BF04-8D5742B32A45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF57CCA-F1B7-E44D-B846-F1C68DEE7B5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="31720" windowHeight="9480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6960" yWindow="2720" windowWidth="31720" windowHeight="9480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -147,9 +147,6 @@
     <t>Text</t>
   </si>
   <si>
-    <t>namemorethan12</t>
-  </si>
-  <si>
     <t>alfSnotBeetl</t>
   </si>
   <si>
@@ -163,6 +160,9 @@
   </si>
   <si>
     <t>Term Type</t>
+  </si>
+  <si>
+    <t>nameismorethan016</t>
   </si>
 </sst>
 </file>
@@ -573,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -650,12 +650,12 @@
         <v>31</v>
       </c>
       <c r="R1" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -683,7 +683,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -695,7 +695,7 @@
         <v>9</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I3" t="s">
         <v>34</v>
@@ -726,7 +726,7 @@
         <v>13</v>
       </c>
       <c r="I4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J4" s="6" t="s">
         <v>10</v>
@@ -773,7 +773,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>9</v>
@@ -800,12 +800,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -987,15 +984,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7613A94-47D1-485D-A76D-D3A6CFAB63B4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4EFE1791-BEC8-419B-A7D8-F7EAC9E3F094}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="aa5be1c8-7296-4b7a-853c-c6802fcefdea"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1019,17 +1027,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4EFE1791-BEC8-419B-A7D8-F7EAC9E3F094}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7613A94-47D1-485D-A76D-D3A6CFAB63B4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="aa5be1c8-7296-4b7a-853c-c6802fcefdea"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>